<commit_message>
Updates to the Shiny app that should make loading and interacting with the app easier. Fixed a couple of fringe cases where BIP would not load correctly. Updated corresponding section of README file.
</commit_message>
<xml_diff>
--- a/inst/IPPO_app/App_backend/example.xlsx
+++ b/inst/IPPO_app/App_backend/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/299755c_curtin_edu_au/Documents/Personal Projects/IPPO App/Outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin-my.sharepoint.com/personal/299755c_curtin_edu_au/Documents/Documents/GitHub/rippo/inst/IPPO_app/App_backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_8E988E9481F1853F7F4CA3FD9A1FBC7DB6A0D2AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5417F7A-57EB-4641-9FDC-F28B5551CE40}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_8E988E9481F1853F7F4CA3FD9A1FBC7DB6A0D2AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD180BBC-2ED6-4231-AA72-D05F72EBE466}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20970" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-9165" windowWidth="21840" windowHeight="37920" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPPO Instructions" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>No.</t>
   </si>
@@ -316,6 +316,16 @@
   </si>
   <si>
     <t>Kate Bens</t>
+  </si>
+  <si>
+    <t>Table 1, Lines 1-4
+Table 2, Lines 1-4
+Table 3, Lines 2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1, Lines 1,2,3
+Table 2, Lines 1:4
+</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1550,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1548,7 +1558,7 @@
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="22.875" customWidth="1"/>
     <col min="3" max="3" width="43.625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
     <col min="6" max="6" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1572,7 +1582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="78.75">
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1586,7 +1596,7 @@
         <v>45658</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>65</v>
@@ -1612,7 +1622,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1625,8 +1635,8 @@
       <c r="D4" s="23">
         <v>46022</v>
       </c>
-      <c r="E4" t="s">
-        <v>69</v>
+      <c r="E4" s="24" t="s">
+        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>65</v>

</xml_diff>